<commit_message>
sistemazione generale perchè sono precisino
</commit_message>
<xml_diff>
--- a/FogliCalcolo/Piping/perdite di carico.xlsx
+++ b/FogliCalcolo/Piping/perdite di carico.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Uni\Impianti meccanici\MaterialeEsame\FogliCalcolo\Piping\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giona\Desktop\git\ImpiantiMeccanici\FogliCalcolo\Piping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7E28F56B-260F-49B2-B903-F2BA9D1116EC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{958771A1-C6EE-49E6-B4EF-1846058B3C14}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1905" yWindow="1905" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Colebrook" sheetId="1" r:id="rId1"/>
@@ -86,21 +86,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="38">
-  <si>
-    <t>Diametro esterno</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="37">
   <si>
     <t>m</t>
   </si>
   <si>
-    <t>Spessore</t>
-  </si>
-  <si>
     <t>diametro interno</t>
-  </si>
-  <si>
-    <t>Lunghezza</t>
   </si>
   <si>
     <t>velocità</t>
@@ -183,9 +174,6 @@
     </r>
   </si>
   <si>
-    <t>Tipo di tubo</t>
-  </si>
-  <si>
     <t>scabrosità relativa</t>
   </si>
   <si>
@@ -224,12 +212,6 @@
     </r>
   </si>
   <si>
-    <t>Fattore di resistenza</t>
-  </si>
-  <si>
-    <t>Eq Colebrook</t>
-  </si>
-  <si>
     <t>cadente</t>
   </si>
   <si>
@@ -246,6 +228,36 @@
   </si>
   <si>
     <t>n</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>Q</t>
+  </si>
+  <si>
+    <t>v</t>
+  </si>
+  <si>
+    <t>l/s</t>
+  </si>
+  <si>
+    <t>km</t>
+  </si>
+  <si>
+    <t>coeff. magg. cadente</t>
+  </si>
+  <si>
+    <t>acciaio internamente bitumato</t>
+  </si>
+  <si>
+    <t>acciaio nuovo zincato</t>
   </si>
   <si>
     <r>
@@ -256,16 +268,7 @@
         <family val="1"/>
         <charset val="2"/>
       </rPr>
-      <t>e</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="18.600000000000001"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>/</t>
+      <t>e/</t>
     </r>
     <r>
       <rPr>
@@ -278,37 +281,22 @@
     </r>
   </si>
   <si>
-    <t>e</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>s</t>
-  </si>
-  <si>
-    <t>Q</t>
-  </si>
-  <si>
-    <t>v</t>
-  </si>
-  <si>
-    <t>l/s</t>
-  </si>
-  <si>
-    <t>Perdita di carico</t>
-  </si>
-  <si>
-    <t>km</t>
-  </si>
-  <si>
-    <t>coeff. magg. cadente</t>
-  </si>
-  <si>
-    <t>acciaio internamente bitumato</t>
-  </si>
-  <si>
-    <t>acciaio nuovo zincato</t>
+    <t>diametro esterno</t>
+  </si>
+  <si>
+    <t>spessore</t>
+  </si>
+  <si>
+    <t>lunghezza</t>
+  </si>
+  <si>
+    <t>tipo di tubo</t>
+  </si>
+  <si>
+    <t>fattore di resistenza</t>
+  </si>
+  <si>
+    <t>eq Colebrook</t>
   </si>
 </sst>
 </file>
@@ -316,17 +304,17 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="9">
-    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="0.0000"/>
-    <numFmt numFmtId="166" formatCode="0.000"/>
-    <numFmt numFmtId="167" formatCode="0.0"/>
-    <numFmt numFmtId="168" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="169" formatCode="_-* #,##0.000_-;\-* #,##0.000_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="170" formatCode="_-* #,##0.0000_-;\-* #,##0.0000_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="171" formatCode="0.000000"/>
-    <numFmt numFmtId="172" formatCode="0.0000000"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="166" formatCode="0.0"/>
+    <numFmt numFmtId="167" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="168" formatCode="_-* #,##0.000_-;\-* #,##0.000_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="169" formatCode="_-* #,##0.0000_-;\-* #,##0.0000_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="170" formatCode="0.000000"/>
+    <numFmt numFmtId="171" formatCode="0.0000000"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -378,12 +366,6 @@
       <charset val="2"/>
     </font>
     <font>
-      <sz val="18.600000000000001"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -409,26 +391,26 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -443,9 +425,12 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="171" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="170" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -454,11 +439,11 @@
     <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -485,15 +470,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>19050</xdr:colOff>
+          <xdr:colOff>43898</xdr:colOff>
           <xdr:row>14</xdr:row>
-          <xdr:rowOff>19050</xdr:rowOff>
+          <xdr:rowOff>43898</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>2</xdr:col>
-          <xdr:colOff>1657</xdr:colOff>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>2387048</xdr:colOff>
           <xdr:row>14</xdr:row>
-          <xdr:rowOff>504825</xdr:rowOff>
+          <xdr:rowOff>529673</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -503,7 +488,7 @@
                   <a14:compatExt spid="_x0000_s1025"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9D6A294F-30FD-444B-905B-28D5F021F1C9}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -540,15 +525,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>942975</xdr:colOff>
+          <xdr:colOff>735911</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>28575</xdr:rowOff>
+          <xdr:rowOff>36858</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>2</xdr:col>
-          <xdr:colOff>1657</xdr:colOff>
-          <xdr:row>16</xdr:row>
-          <xdr:rowOff>9525</xdr:rowOff>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>1838741</xdr:colOff>
+          <xdr:row>15</xdr:row>
+          <xdr:rowOff>523047</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -558,7 +543,7 @@
                   <a14:compatExt spid="_x0000_s1026"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{587C52CE-72CC-41A8-AF56-6CD026E0FCB9}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -595,15 +580,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>1019175</xdr:colOff>
+          <xdr:colOff>919784</xdr:colOff>
           <xdr:row>12</xdr:row>
-          <xdr:rowOff>47625</xdr:rowOff>
+          <xdr:rowOff>39342</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>2286000</xdr:colOff>
+          <xdr:colOff>1722782</xdr:colOff>
           <xdr:row>12</xdr:row>
-          <xdr:rowOff>504825</xdr:rowOff>
+          <xdr:rowOff>442736</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -613,7 +598,7 @@
                   <a14:compatExt spid="_x0000_s1027"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6A2EA4EA-22B6-4C70-8E4F-80F8FEAD57BD}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -650,15 +635,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>1095375</xdr:colOff>
+          <xdr:colOff>896593</xdr:colOff>
           <xdr:row>13</xdr:row>
-          <xdr:rowOff>28575</xdr:rowOff>
+          <xdr:rowOff>36857</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>2286000</xdr:colOff>
-          <xdr:row>14</xdr:row>
-          <xdr:rowOff>3313</xdr:rowOff>
+          <xdr:colOff>1764197</xdr:colOff>
+          <xdr:row>13</xdr:row>
+          <xdr:rowOff>620930</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -668,7 +653,7 @@
                   <a14:compatExt spid="_x0000_s1028"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BF3F94C8-C997-4147-9CFE-D6FC1FD12774}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -710,15 +695,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>85725</xdr:colOff>
+          <xdr:colOff>71071</xdr:colOff>
           <xdr:row>9</xdr:row>
           <xdr:rowOff>28575</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>2</xdr:col>
-          <xdr:colOff>2931</xdr:colOff>
-          <xdr:row>10</xdr:row>
-          <xdr:rowOff>0</xdr:rowOff>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>1299796</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>476250</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -728,7 +713,7 @@
                   <a14:compatExt spid="_x0000_s2053"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{78907331-4CF2-415E-A58E-ECAF065E385D}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000005080000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -770,15 +755,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>19050</xdr:colOff>
+          <xdr:colOff>48358</xdr:colOff>
           <xdr:row>9</xdr:row>
-          <xdr:rowOff>19050</xdr:rowOff>
+          <xdr:rowOff>33704</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>2</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
-          <xdr:row>10</xdr:row>
-          <xdr:rowOff>0</xdr:rowOff>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>1553308</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>490904</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -788,7 +773,7 @@
                   <a14:compatExt spid="_x0000_s3073"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{43E4B16B-2439-47CA-BEDC-3CD410875700}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-0000010C0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1147,26 +1132,26 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.7109375" customWidth="1"/>
-    <col min="2" max="2" width="35.42578125" style="11" customWidth="1"/>
-    <col min="3" max="3" width="4.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.42578125" style="11" customWidth="1"/>
+    <col min="3" max="3" width="5.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D1" s="2">
         <v>1</v>
@@ -1174,13 +1159,13 @@
     </row>
     <row r="2" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D2" s="2">
         <f>+D1*D7</f>
@@ -1189,10 +1174,10 @@
     </row>
     <row r="3" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D3" s="4">
         <f>+D2*3600</f>
@@ -1201,10 +1186,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>0</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>1</v>
       </c>
       <c r="D4" s="2">
         <v>0.108</v>
@@ -1212,13 +1197,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>2</v>
+        <v>32</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D5" s="2">
         <v>3.5999999999999999E-3</v>
@@ -1226,13 +1211,13 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D6" s="2">
         <f>+D4-2*D5</f>
@@ -1241,10 +1226,10 @@
     </row>
     <row r="7" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D7" s="7">
         <f>+PI()*(D6^2)/4</f>
@@ -1253,10 +1238,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>4</v>
+        <v>33</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D8" s="6">
         <v>1000</v>
@@ -1264,57 +1249,59 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" s="21" t="s">
-        <v>36</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="B9" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="24"/>
+      <c r="D9" s="24"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D10" s="15">
+        <v>0</v>
+      </c>
+      <c r="D10" s="21">
         <f>0.1/1000</f>
         <v>1E-4</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="24.75" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="D11" s="2">
+        <v>9</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="22">
         <f>+D10/(D6)</f>
         <v>9.9206349206349201E-4</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" s="16">
+        <v>13</v>
+      </c>
+      <c r="D12" s="23">
         <f>1.24*10^-6</f>
         <v>1.24E-6</v>
       </c>
     </row>
-    <row r="13" spans="1:4" s="8" customFormat="1" ht="40.35" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" s="8" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B13" s="13"/>
       <c r="C13" s="9"/>
@@ -1323,9 +1310,9 @@
         <v>81290.322580645166</v>
       </c>
     </row>
-    <row r="14" spans="1:4" s="8" customFormat="1" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" s="8" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="B14" s="13"/>
       <c r="C14" s="9"/>
@@ -1333,9 +1320,9 @@
         <v>2.2608000334446501E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:4" s="8" customFormat="1" ht="40.35" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" s="8" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="B15" s="13"/>
       <c r="C15" s="9"/>
@@ -1344,13 +1331,13 @@
         <v>-3.3762175899454405E-7</v>
       </c>
     </row>
-    <row r="16" spans="1:4" s="8" customFormat="1" ht="40.35" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" s="8" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B16" s="13"/>
       <c r="C16" s="9" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="D16" s="17">
         <f>+D14*(D1^2)/2/9.81/D6</f>
@@ -1359,10 +1346,10 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D17" s="3">
         <f>+D16*D8</f>
@@ -1370,6 +1357,9 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B9:D9"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -1378,19 +1368,19 @@
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
         <oleObject progId="Equation.3" shapeId="1025" r:id="rId4">
-          <objectPr defaultSize="0" r:id="rId5">
+          <objectPr defaultSize="0" autoPict="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>1</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
+                <xdr:colOff>47625</xdr:colOff>
                 <xdr:row>14</xdr:row>
-                <xdr:rowOff>19050</xdr:rowOff>
+                <xdr:rowOff>47625</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>1</xdr:col>
-                <xdr:colOff>3371850</xdr:colOff>
+                <xdr:colOff>2390775</xdr:colOff>
                 <xdr:row>14</xdr:row>
-                <xdr:rowOff>657225</xdr:rowOff>
+                <xdr:rowOff>533400</xdr:rowOff>
               </to>
             </anchor>
           </objectPr>
@@ -1403,19 +1393,19 @@
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
         <oleObject progId="Equation.3" shapeId="1026" r:id="rId6">
-          <objectPr defaultSize="0" r:id="rId7">
+          <objectPr defaultSize="0" autoPict="0" r:id="rId7">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>1</xdr:col>
-                <xdr:colOff>942975</xdr:colOff>
+                <xdr:colOff>733425</xdr:colOff>
                 <xdr:row>15</xdr:row>
-                <xdr:rowOff>28575</xdr:rowOff>
+                <xdr:rowOff>38100</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>1</xdr:col>
-                <xdr:colOff>2428875</xdr:colOff>
-                <xdr:row>16</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
+                <xdr:colOff>1838325</xdr:colOff>
+                <xdr:row>15</xdr:row>
+                <xdr:rowOff>523875</xdr:rowOff>
               </to>
             </anchor>
           </objectPr>
@@ -1428,19 +1418,19 @@
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
         <oleObject progId="Equation.3" shapeId="1027" r:id="rId8">
-          <objectPr defaultSize="0" r:id="rId9">
+          <objectPr defaultSize="0" autoPict="0" r:id="rId9">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>1</xdr:col>
-                <xdr:colOff>1019175</xdr:colOff>
+                <xdr:colOff>923925</xdr:colOff>
                 <xdr:row>12</xdr:row>
-                <xdr:rowOff>47625</xdr:rowOff>
+                <xdr:rowOff>38100</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>1</xdr:col>
-                <xdr:colOff>2286000</xdr:colOff>
+                <xdr:colOff>1724025</xdr:colOff>
                 <xdr:row>12</xdr:row>
-                <xdr:rowOff>647700</xdr:rowOff>
+                <xdr:rowOff>438150</xdr:rowOff>
               </to>
             </anchor>
           </objectPr>
@@ -1453,19 +1443,19 @@
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
         <oleObject progId="Equation.3" shapeId="1028" r:id="rId10">
-          <objectPr defaultSize="0" r:id="rId11">
+          <objectPr defaultSize="0" autoPict="0" r:id="rId11">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>1</xdr:col>
-                <xdr:colOff>1095375</xdr:colOff>
+                <xdr:colOff>895350</xdr:colOff>
                 <xdr:row>13</xdr:row>
-                <xdr:rowOff>28575</xdr:rowOff>
+                <xdr:rowOff>38100</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>1</xdr:col>
-                <xdr:colOff>2286000</xdr:colOff>
+                <xdr:colOff>1762125</xdr:colOff>
                 <xdr:row>13</xdr:row>
-                <xdr:rowOff>914400</xdr:rowOff>
+                <xdr:rowOff>619125</xdr:rowOff>
               </to>
             </anchor>
           </objectPr>
@@ -1484,26 +1474,26 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.7109375" customWidth="1"/>
-    <col min="2" max="2" width="19.7109375" style="11" customWidth="1"/>
-    <col min="3" max="3" width="8.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" style="11" customWidth="1"/>
+    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D1" s="2">
         <v>1</v>
@@ -1511,13 +1501,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="D2" s="2">
         <f>+D1*D7*1000</f>
@@ -1526,10 +1516,10 @@
     </row>
     <row r="3" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D3" s="4">
         <f>+D2*3.6</f>
@@ -1538,10 +1528,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D4" s="2">
         <v>108</v>
@@ -1549,13 +1539,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>2</v>
+        <v>32</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D5" s="2">
         <v>3.6</v>
@@ -1563,13 +1553,13 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D6" s="2">
         <f>+D4-2*D5</f>
@@ -1578,10 +1568,10 @@
     </row>
     <row r="7" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D7" s="7">
         <f>+PI()*(D6^2)/4/1000000</f>
@@ -1590,10 +1580,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>4</v>
+        <v>33</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="D8" s="6">
         <v>1</v>
@@ -1601,19 +1591,21 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" s="21" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" s="8" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+      <c r="B9" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="24"/>
+      <c r="D9" s="24"/>
+    </row>
+    <row r="10" spans="1:4" s="8" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B10" s="13"/>
       <c r="C10" s="9" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D10" s="19">
         <f>6.81*10^8*D2^1.82*D4^-4.71</f>
@@ -1622,7 +1614,7 @@
     </row>
     <row r="11" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="B11" s="13"/>
       <c r="C11" s="9"/>
@@ -1632,10 +1624,10 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D12" s="3">
         <f>+D10*D8*D11</f>
@@ -1653,22 +1645,22 @@
       <c r="B15" s="12"/>
       <c r="D15" s="16"/>
     </row>
-    <row r="16" spans="1:4" s="8" customFormat="1" ht="40.35" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B16" s="13"/>
       <c r="C16" s="9"/>
       <c r="D16" s="18"/>
     </row>
-    <row r="17" spans="2:4" s="8" customFormat="1" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B17" s="13"/>
       <c r="C17" s="9"/>
       <c r="D17" s="20"/>
     </row>
-    <row r="18" spans="2:4" s="8" customFormat="1" ht="40.35" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B18" s="13"/>
       <c r="C18" s="9"/>
       <c r="D18" s="10"/>
     </row>
-    <row r="19" spans="2:4" s="8" customFormat="1" ht="40.35" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B19" s="13"/>
       <c r="C19" s="9"/>
       <c r="D19" s="17"/>
@@ -1677,6 +1669,9 @@
       <c r="D20" s="3"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B9:D9"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -1685,19 +1680,19 @@
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
         <oleObject progId="Equation.3" shapeId="2053" r:id="rId4">
-          <objectPr defaultSize="0" r:id="rId5">
+          <objectPr defaultSize="0" autoPict="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>1</xdr:col>
-                <xdr:colOff>85725</xdr:colOff>
+                <xdr:colOff>66675</xdr:colOff>
                 <xdr:row>9</xdr:row>
                 <xdr:rowOff>28575</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>1</xdr:col>
-                <xdr:colOff>1676400</xdr:colOff>
+                <xdr:colOff>1295400</xdr:colOff>
                 <xdr:row>9</xdr:row>
-                <xdr:rowOff>571500</xdr:rowOff>
+                <xdr:rowOff>476250</xdr:rowOff>
               </to>
             </anchor>
           </objectPr>
@@ -1716,26 +1711,26 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.7109375" customWidth="1"/>
-    <col min="2" max="2" width="22.85546875" style="11" customWidth="1"/>
-    <col min="3" max="3" width="4.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24" style="11" customWidth="1"/>
+    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D1" s="4">
         <v>1</v>
@@ -1743,13 +1738,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="D2" s="3">
         <f>+D1*D7*1000</f>
@@ -1758,10 +1753,10 @@
     </row>
     <row r="3" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D3" s="4">
         <f>+D2*3.6</f>
@@ -1770,10 +1765,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D4" s="5">
         <v>108</v>
@@ -1781,13 +1776,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>2</v>
+        <v>32</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D5" s="5">
         <v>3.6</v>
@@ -1795,13 +1790,13 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D6" s="5">
         <f>+D4-2*D5</f>
@@ -1810,10 +1805,10 @@
     </row>
     <row r="7" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D7" s="7">
         <f>+PI()*(D6^2)/4/1000000</f>
@@ -1822,10 +1817,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>4</v>
+        <v>33</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="D8" s="6">
         <v>1</v>
@@ -1833,19 +1828,21 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" s="21" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" s="8" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+      <c r="B9" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="24"/>
+      <c r="D9" s="24"/>
+    </row>
+    <row r="10" spans="1:4" s="8" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B10" s="13"/>
       <c r="C10" s="9" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D10" s="19">
         <f>6.81*10^8*D2^1.83*D4^-4.83</f>
@@ -1854,7 +1851,7 @@
     </row>
     <row r="11" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="B11" s="13"/>
       <c r="C11" s="9"/>
@@ -1864,10 +1861,10 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D12" s="3">
         <f>+D10*D8*D11</f>
@@ -1878,29 +1875,29 @@
       <c r="B13" s="12"/>
       <c r="D13" s="15"/>
     </row>
-    <row r="14" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="14"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B15" s="12"/>
       <c r="D15" s="16"/>
     </row>
-    <row r="16" spans="1:4" s="8" customFormat="1" ht="40.35" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B16" s="13"/>
       <c r="C16" s="9"/>
       <c r="D16" s="18"/>
     </row>
-    <row r="17" spans="2:4" s="8" customFormat="1" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B17" s="13"/>
       <c r="C17" s="9"/>
       <c r="D17" s="20"/>
     </row>
-    <row r="18" spans="2:4" s="8" customFormat="1" ht="40.35" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B18" s="13"/>
       <c r="C18" s="9"/>
       <c r="D18" s="10"/>
     </row>
-    <row r="19" spans="2:4" s="8" customFormat="1" ht="40.35" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B19" s="13"/>
       <c r="C19" s="9"/>
       <c r="D19" s="17"/>
@@ -1909,6 +1906,9 @@
       <c r="D20" s="3"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B9:D9"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -1917,19 +1917,19 @@
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
         <oleObject progId="Equation.3" shapeId="3073" r:id="rId4">
-          <objectPr defaultSize="0" r:id="rId5">
+          <objectPr defaultSize="0" autoPict="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>1</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
+                <xdr:colOff>47625</xdr:colOff>
                 <xdr:row>9</xdr:row>
-                <xdr:rowOff>19050</xdr:rowOff>
+                <xdr:rowOff>38100</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>1</xdr:col>
-                <xdr:colOff>2133600</xdr:colOff>
-                <xdr:row>10</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
+                <xdr:colOff>1552575</xdr:colOff>
+                <xdr:row>9</xdr:row>
+                <xdr:rowOff>495300</xdr:rowOff>
               </to>
             </anchor>
           </objectPr>

</xml_diff>